<commit_message>
Combine stages of pre-processing to eliminate redundant files
</commit_message>
<xml_diff>
--- a/data/co2/co2_data_raw.xlsx
+++ b/data/co2/co2_data_raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate\Documents\AI4GoodLab\carbon-footprint-tracker\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate\Documents\AI4GoodLab\carbon-footprint-tracker\data\co2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01C5E1-92AA-4FD4-8FD8-B9DF5D15A314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE105403-6A2F-4935-8572-07DB83D460D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="425">
   <si>
     <t>n</t>
   </si>
@@ -1345,6 +1345,12 @@
   </si>
   <si>
     <t>GREEN BEAN fresh</t>
+  </si>
+  <si>
+    <t>BEEF WITH BONE</t>
+  </si>
+  <si>
+    <t>BEEF BONELESS</t>
   </si>
 </sst>
 </file>
@@ -1878,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C207" sqref="C207"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8368,7 +8374,7 @@
     </row>
     <row r="102" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
-        <v>156</v>
+        <v>424</v>
       </c>
       <c r="B102" s="11"/>
       <c r="C102" s="12" t="s">
@@ -8430,7 +8436,7 @@
     </row>
     <row r="103" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>157</v>
+        <v>423</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
word simplification in co2 dataset
</commit_message>
<xml_diff>
--- a/data/co2/co2_data_raw.xlsx
+++ b/data/co2/co2_data_raw.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate\Documents\AI4GoodLab\carbon-footprint-tracker\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kate\Documents\AI4GoodLab\carbon-footprint-tracker\data\co2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01C5E1-92AA-4FD4-8FD8-B9DF5D15A314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766E2B1A-6520-41E3-A222-15C85FBAC793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="430">
   <si>
     <t>n</t>
   </si>
@@ -666,33 +666,12 @@
     <t>POULTRY BONE FREE MEAT</t>
   </si>
   <si>
-    <t>CHICKEN BONE FREE MEAT</t>
-  </si>
-  <si>
-    <t>EMU BONE FREE MEAT</t>
-  </si>
-  <si>
-    <t>DUCK MEAT BONE FREE</t>
-  </si>
-  <si>
-    <t>TURKEY MEAT BONE FREE</t>
-  </si>
-  <si>
     <t>ITEM or TYPOLOGY</t>
   </si>
   <si>
     <t>POULTRY MEAT WITH BONE</t>
   </si>
   <si>
-    <t>CHICKEN MEAT WITH BONE</t>
-  </si>
-  <si>
-    <t>DUCK MEAT WITH BONE</t>
-  </si>
-  <si>
-    <t>TURKEY MEAT WITH BONE</t>
-  </si>
-  <si>
     <t>RABBIT MEAT WITH BONE*</t>
   </si>
   <si>
@@ -708,9 +687,6 @@
     <t>YOGURT LACTOSE FREE</t>
   </si>
   <si>
-    <t>YOGURT WHITE</t>
-  </si>
-  <si>
     <t>COFFEE GREEN*</t>
   </si>
   <si>
@@ -1335,16 +1311,61 @@
     <t>CHILI</t>
   </si>
   <si>
-    <t>SHRIMPS (F)</t>
-  </si>
-  <si>
-    <t>SHRIMPS</t>
-  </si>
-  <si>
     <t>GREEN BEAN fresh (g)*</t>
   </si>
   <si>
     <t>GREEN BEAN fresh</t>
+  </si>
+  <si>
+    <t>SHRIMP (F)</t>
+  </si>
+  <si>
+    <t>SHRIMP</t>
+  </si>
+  <si>
+    <t>YOGURT PLAIN</t>
+  </si>
+  <si>
+    <t>PORK</t>
+  </si>
+  <si>
+    <t>CHICKEN BONELESS</t>
+  </si>
+  <si>
+    <t>EMU BONELESS</t>
+  </si>
+  <si>
+    <t>DUCK BONELESS</t>
+  </si>
+  <si>
+    <t>TURKEY BONELESS</t>
+  </si>
+  <si>
+    <t>DUCK</t>
+  </si>
+  <si>
+    <t>CHICKEN</t>
+  </si>
+  <si>
+    <t>TURKEY</t>
+  </si>
+  <si>
+    <t>RABBIT</t>
+  </si>
+  <si>
+    <t>LAMB</t>
+  </si>
+  <si>
+    <t>LAMB BONELESS</t>
+  </si>
+  <si>
+    <t>BEEF BONELESS</t>
+  </si>
+  <si>
+    <t>BEEF</t>
+  </si>
+  <si>
+    <t>BUFFALO BONELESS</t>
   </si>
 </sst>
 </file>
@@ -1878,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C207" sqref="C207"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,13 +1931,13 @@
   <sheetData>
     <row r="1" spans="1:24" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -3516,7 +3537,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="D26" s="13">
         <v>1</v>
@@ -8372,7 +8393,7 @@
       </c>
       <c r="B102" s="11"/>
       <c r="C102" s="12" t="s">
-        <v>156</v>
+        <v>427</v>
       </c>
       <c r="D102" s="13">
         <v>183</v>
@@ -8436,7 +8457,7 @@
         <v>18</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>157</v>
+        <v>428</v>
       </c>
       <c r="D103" s="13">
         <v>172</v>
@@ -8500,7 +8521,7 @@
         <v>18</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>158</v>
+        <v>429</v>
       </c>
       <c r="D104" s="13">
         <v>3</v>
@@ -9834,7 +9855,7 @@
         <v>18</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>182</v>
+        <v>426</v>
       </c>
       <c r="D125" s="13">
         <v>55</v>
@@ -9898,7 +9919,7 @@
         <v>18</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>183</v>
+        <v>425</v>
       </c>
       <c r="D126" s="13">
         <v>55</v>
@@ -10154,7 +10175,7 @@
         <v>18</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>188</v>
+        <v>416</v>
       </c>
       <c r="D130" s="13">
         <v>135</v>
@@ -10474,7 +10495,7 @@
         <v>18</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>194</v>
+        <v>416</v>
       </c>
       <c r="D135" s="13">
         <v>131</v>
@@ -10538,7 +10559,7 @@
         <v>18</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>196</v>
+        <v>417</v>
       </c>
       <c r="D136" s="13">
         <v>100</v>
@@ -10602,7 +10623,7 @@
         <v>18</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>197</v>
+        <v>418</v>
       </c>
       <c r="D137" s="13">
         <v>1</v>
@@ -10664,7 +10685,7 @@
       </c>
       <c r="B138" s="11"/>
       <c r="C138" s="12" t="s">
-        <v>198</v>
+        <v>419</v>
       </c>
       <c r="D138" s="13">
         <v>1</v>
@@ -10724,7 +10745,7 @@
       </c>
       <c r="B139" s="11"/>
       <c r="C139" s="12" t="s">
-        <v>199</v>
+        <v>420</v>
       </c>
       <c r="D139" s="13">
         <v>12</v>
@@ -10775,20 +10796,20 @@
         <v>20</v>
       </c>
       <c r="T139" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U139" s="12"/>
       <c r="V139" s="20"/>
     </row>
     <row r="140" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B140" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>202</v>
+        <v>422</v>
       </c>
       <c r="D140" s="13">
         <v>98</v>
@@ -10846,13 +10867,13 @@
     </row>
     <row r="141" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B141" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>203</v>
+        <v>421</v>
       </c>
       <c r="D141" s="13">
         <v>1</v>
@@ -10910,13 +10931,13 @@
     </row>
     <row r="142" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="12" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B142" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>204</v>
+        <v>423</v>
       </c>
       <c r="D142" s="13">
         <v>6</v>
@@ -10974,13 +10995,13 @@
     </row>
     <row r="143" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B143" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>205</v>
+        <v>424</v>
       </c>
       <c r="D143" s="13">
         <v>2</v>
@@ -11038,13 +11059,13 @@
     </row>
     <row r="144" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B144" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D144" s="13">
         <v>1</v>
@@ -11102,13 +11123,13 @@
     </row>
     <row r="145" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B145" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D145" s="13">
         <v>14</v>
@@ -11166,13 +11187,13 @@
     </row>
     <row r="146" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B146" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D146" s="13">
         <v>4</v>
@@ -11223,20 +11244,20 @@
         <v>27</v>
       </c>
       <c r="T146" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U146" s="12"/>
       <c r="V146" s="20"/>
     </row>
     <row r="147" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B147" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>210</v>
+        <v>415</v>
       </c>
       <c r="D147" s="13">
         <v>20</v>
@@ -11294,13 +11315,13 @@
     </row>
     <row r="148" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B148" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D148" s="13">
         <v>8</v>
@@ -11358,13 +11379,13 @@
     </row>
     <row r="149" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="12" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B149" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D149" s="13">
         <v>2</v>
@@ -11422,13 +11443,13 @@
     </row>
     <row r="150" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="12" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B150" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D150" s="13">
         <v>5</v>
@@ -11486,13 +11507,13 @@
     </row>
     <row r="151" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="12" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D151" s="13">
         <v>1</v>
@@ -11550,13 +11571,13 @@
     </row>
     <row r="152" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D152" s="13">
         <v>2</v>
@@ -11614,13 +11635,13 @@
     </row>
     <row r="153" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="12" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B153" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D153" s="13">
         <v>4</v>
@@ -11678,13 +11699,13 @@
     </row>
     <row r="154" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B154" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D154" s="13">
         <v>4</v>
@@ -11742,13 +11763,13 @@
     </row>
     <row r="155" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B155" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D155" s="13">
         <v>20</v>
@@ -11806,13 +11827,13 @@
     </row>
     <row r="156" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B156" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D156" s="13">
         <v>1</v>
@@ -11870,13 +11891,13 @@
     </row>
     <row r="157" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B157" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D157" s="13">
         <v>1</v>
@@ -11934,13 +11955,13 @@
     </row>
     <row r="158" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B158" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D158" s="13">
         <v>7</v>
@@ -11998,13 +12019,13 @@
     </row>
     <row r="159" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B159" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D159" s="13">
         <v>1</v>
@@ -12062,13 +12083,13 @@
     </row>
     <row r="160" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B160" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D160" s="13">
         <v>2</v>
@@ -12126,13 +12147,13 @@
     </row>
     <row r="161" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="12" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B161" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D161" s="13">
         <v>4</v>
@@ -12190,13 +12211,13 @@
     </row>
     <row r="162" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D162" s="13">
         <v>3</v>
@@ -12252,13 +12273,13 @@
     </row>
     <row r="163" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D163" s="13">
         <v>2</v>
@@ -12316,13 +12337,13 @@
     </row>
     <row r="164" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D164" s="13">
         <v>2</v>
@@ -12380,13 +12401,13 @@
     </row>
     <row r="165" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D165" s="13">
         <v>7</v>
@@ -12444,13 +12465,13 @@
     </row>
     <row r="166" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D166" s="13">
         <v>31</v>
@@ -12508,13 +12529,13 @@
     </row>
     <row r="167" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D167" s="13">
         <v>1</v>
@@ -12572,13 +12593,13 @@
     </row>
     <row r="168" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C168" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="B168" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="C168" s="12" t="s">
-        <v>237</v>
       </c>
       <c r="D168" s="13">
         <v>2</v>
@@ -12636,13 +12657,13 @@
     </row>
     <row r="169" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B169" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D169" s="13">
         <v>59</v>
@@ -12700,13 +12721,13 @@
     </row>
     <row r="170" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D170" s="13">
         <v>7</v>
@@ -12764,13 +12785,13 @@
     </row>
     <row r="171" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C171" s="12" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D171" s="13">
         <v>4</v>
@@ -12828,13 +12849,13 @@
     </row>
     <row r="172" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D172" s="13">
         <v>9</v>
@@ -12892,13 +12913,13 @@
     </row>
     <row r="173" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="D173" s="13">
         <v>2</v>
@@ -12956,13 +12977,13 @@
     </row>
     <row r="174" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D174" s="13">
         <v>7</v>
@@ -13020,13 +13041,13 @@
     </row>
     <row r="175" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D175" s="13">
         <v>3</v>
@@ -13082,13 +13103,13 @@
     </row>
     <row r="176" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D176" s="13">
         <v>15</v>
@@ -13146,13 +13167,13 @@
     </row>
     <row r="177" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B177" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C177" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="C177" s="12" t="s">
-        <v>246</v>
       </c>
       <c r="D177" s="13">
         <v>1</v>
@@ -13210,13 +13231,13 @@
     </row>
     <row r="178" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D178" s="13">
         <v>12</v>
@@ -13274,13 +13295,13 @@
     </row>
     <row r="179" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D179" s="13">
         <v>6</v>
@@ -13338,13 +13359,13 @@
     </row>
     <row r="180" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D180" s="13">
         <v>6</v>
@@ -13402,13 +13423,13 @@
     </row>
     <row r="181" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C181" s="12" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="D181" s="13">
         <v>12</v>
@@ -13466,13 +13487,13 @@
     </row>
     <row r="182" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D182" s="13">
         <v>12</v>
@@ -13530,13 +13551,13 @@
     </row>
     <row r="183" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D183" s="13">
         <v>6</v>
@@ -13587,20 +13608,20 @@
         <v>27</v>
       </c>
       <c r="T183" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U183" s="12"/>
       <c r="V183" s="20"/>
     </row>
     <row r="184" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D184" s="13">
         <v>3</v>
@@ -13656,13 +13677,13 @@
     </row>
     <row r="185" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D185" s="13">
         <v>3</v>
@@ -13718,13 +13739,13 @@
     </row>
     <row r="186" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D186" s="13">
         <v>1</v>
@@ -13782,13 +13803,13 @@
     </row>
     <row r="187" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C187" s="12" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D187" s="13">
         <v>1</v>
@@ -13846,13 +13867,13 @@
     </row>
     <row r="188" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C188" s="12" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D188" s="13">
         <v>9</v>
@@ -13910,13 +13931,13 @@
     </row>
     <row r="189" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B189" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D189" s="13">
         <v>1</v>
@@ -13974,13 +13995,13 @@
     </row>
     <row r="190" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B190" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="D190" s="13">
         <v>8</v>
@@ -14038,13 +14059,13 @@
     </row>
     <row r="191" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B191" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D191" s="13">
         <v>3</v>
@@ -14100,13 +14121,13 @@
     </row>
     <row r="192" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B192" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D192" s="13">
         <v>2</v>
@@ -14164,13 +14185,13 @@
     </row>
     <row r="193" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B193" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D193" s="13">
         <v>1</v>
@@ -14228,13 +14249,13 @@
     </row>
     <row r="194" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B194" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D194" s="13">
         <v>2</v>
@@ -14292,13 +14313,13 @@
     </row>
     <row r="195" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="12" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B195" s="11" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D195" s="13">
         <v>27</v>
@@ -14356,13 +14377,13 @@
     </row>
     <row r="196" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B196" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D196" s="13">
         <v>17</v>
@@ -14420,13 +14441,13 @@
     </row>
     <row r="197" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B197" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D197" s="13">
         <v>7</v>
@@ -14477,20 +14498,20 @@
         <v>27</v>
       </c>
       <c r="T197" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U197" s="12"/>
       <c r="V197" s="20"/>
     </row>
     <row r="198" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B198" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D198" s="13">
         <v>2</v>
@@ -14548,13 +14569,13 @@
     </row>
     <row r="199" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B199" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D199" s="13">
         <v>5</v>
@@ -14612,13 +14633,13 @@
     </row>
     <row r="200" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B200" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D200" s="13">
         <v>12</v>
@@ -14676,13 +14697,13 @@
     </row>
     <row r="201" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B201" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D201" s="13">
         <v>3</v>
@@ -14738,13 +14759,13 @@
     </row>
     <row r="202" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="12" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B202" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D202" s="13">
         <v>1</v>
@@ -14802,13 +14823,13 @@
     </row>
     <row r="203" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B203" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C203" s="12" t="s">
         <v>267</v>
-      </c>
-      <c r="B203" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C203" s="12" t="s">
-        <v>275</v>
       </c>
       <c r="D203" s="13">
         <v>44</v>
@@ -14866,13 +14887,13 @@
     </row>
     <row r="204" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B204" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D204" s="13">
         <v>14</v>
@@ -14930,13 +14951,13 @@
     </row>
     <row r="205" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B205" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D205" s="13">
         <v>3</v>
@@ -14992,13 +15013,13 @@
     </row>
     <row r="206" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B206" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C206" s="12" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D206" s="13">
         <v>4</v>
@@ -15056,13 +15077,13 @@
     </row>
     <row r="207" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B207" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D207" s="13">
         <v>11</v>
@@ -15120,13 +15141,13 @@
     </row>
     <row r="208" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B208" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C208" s="12" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D208" s="13">
         <v>2</v>
@@ -15184,13 +15205,13 @@
     </row>
     <row r="209" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B209" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D209" s="13">
         <v>12</v>
@@ -15248,13 +15269,13 @@
     </row>
     <row r="210" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="12" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B210" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D210" s="13">
         <v>5</v>
@@ -15312,13 +15333,13 @@
     </row>
     <row r="211" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="12" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B211" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="D211" s="13">
         <v>4</v>
@@ -15376,11 +15397,11 @@
     </row>
     <row r="212" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="12" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B212" s="11"/>
       <c r="C212" s="12" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D212" s="13">
         <v>6</v>
@@ -15438,13 +15459,13 @@
     </row>
     <row r="213" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B213" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D213" s="13">
         <v>13</v>
@@ -15502,13 +15523,13 @@
     </row>
     <row r="214" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B214" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D214" s="13">
         <v>11</v>
@@ -15566,13 +15587,13 @@
     </row>
     <row r="215" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B215" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D215" s="13">
         <v>3</v>
@@ -15628,13 +15649,13 @@
     </row>
     <row r="216" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B216" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D216" s="13">
         <v>5</v>
@@ -15692,13 +15713,13 @@
     </row>
     <row r="217" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B217" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C217" s="12" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D217" s="13">
         <v>1</v>
@@ -15756,13 +15777,13 @@
     </row>
     <row r="218" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B218" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D218" s="13">
         <v>1</v>
@@ -15820,13 +15841,13 @@
     </row>
     <row r="219" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B219" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C219" s="12" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D219" s="13">
         <v>10</v>
@@ -15884,13 +15905,13 @@
     </row>
     <row r="220" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B220" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C220" s="12" t="s">
         <v>285</v>
-      </c>
-      <c r="B220" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C220" s="12" t="s">
-        <v>293</v>
       </c>
       <c r="D220" s="13">
         <v>4</v>
@@ -15948,13 +15969,13 @@
     </row>
     <row r="221" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B221" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D221" s="13">
         <v>5</v>
@@ -16012,13 +16033,13 @@
     </row>
     <row r="222" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B222" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C222" s="12" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D222" s="13">
         <v>35</v>
@@ -16076,13 +16097,13 @@
     </row>
     <row r="223" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="12" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B223" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C223" s="12" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D223" s="13">
         <v>3</v>
@@ -16138,13 +16159,13 @@
     </row>
     <row r="224" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="12" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B224" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C224" s="12" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D224" s="13">
         <v>1</v>
@@ -16202,13 +16223,13 @@
     </row>
     <row r="225" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="12" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B225" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D225" s="13">
         <v>2</v>
@@ -16266,13 +16287,13 @@
     </row>
     <row r="226" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="12" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B226" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="D226" s="13">
         <v>1</v>
@@ -16330,13 +16351,13 @@
     </row>
     <row r="227" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="12" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B227" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D227" s="13">
         <v>1</v>
@@ -16394,13 +16415,13 @@
     </row>
     <row r="228" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="12" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B228" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="D228" s="13">
         <v>35</v>
@@ -16458,13 +16479,13 @@
     </row>
     <row r="229" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="12" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B229" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="D229" s="13">
         <v>2</v>
@@ -16522,13 +16543,13 @@
     </row>
     <row r="230" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B230" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D230" s="13">
         <v>3</v>
@@ -16584,13 +16605,13 @@
     </row>
     <row r="231" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="12" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B231" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C231" s="12" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D231" s="13">
         <v>8</v>
@@ -16648,13 +16669,13 @@
     </row>
     <row r="232" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="12" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B232" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D232" s="13">
         <v>4</v>
@@ -16705,20 +16726,20 @@
         <v>27</v>
       </c>
       <c r="T232" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="U232" s="12"/>
       <c r="V232" s="20"/>
     </row>
     <row r="233" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="12" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B233" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C233" s="12" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D233" s="13">
         <v>7</v>
@@ -16776,13 +16797,13 @@
     </row>
     <row r="234" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="12" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B234" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C234" s="12" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D234" s="13">
         <v>4</v>
@@ -16840,13 +16861,13 @@
     </row>
     <row r="235" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="12" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B235" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D235" s="13">
         <v>36</v>
@@ -16904,13 +16925,13 @@
     </row>
     <row r="236" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="12" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B236" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D236" s="13">
         <v>1</v>
@@ -16968,13 +16989,13 @@
     </row>
     <row r="237" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="12" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B237" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C237" s="12" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D237" s="13">
         <v>1</v>
@@ -17032,13 +17053,13 @@
     </row>
     <row r="238" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="12" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B238" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D238" s="13">
         <v>2</v>
@@ -17096,13 +17117,13 @@
     </row>
     <row r="239" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="12" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B239" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D239" s="13">
         <v>28</v>
@@ -17160,13 +17181,13 @@
     </row>
     <row r="240" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="12" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B240" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D240" s="13">
         <v>2</v>
@@ -17224,13 +17245,13 @@
     </row>
     <row r="241" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B241" s="11" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C241" s="12" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D241" s="13">
         <v>33</v>
@@ -17288,13 +17309,13 @@
     </row>
     <row r="242" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B242" s="11" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C242" s="12" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D242" s="13">
         <v>9</v>
@@ -17352,13 +17373,13 @@
     </row>
     <row r="243" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B243" s="11" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C243" s="12" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D243" s="13">
         <v>27</v>
@@ -17416,13 +17437,13 @@
     </row>
     <row r="244" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B244" s="11" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C244" s="12" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D244" s="13">
         <v>4</v>
@@ -17480,13 +17501,13 @@
     </row>
     <row r="245" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="B245" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C245" s="12" t="s">
         <v>318</v>
-      </c>
-      <c r="B245" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="C245" s="12" t="s">
-        <v>326</v>
       </c>
       <c r="D245" s="13">
         <v>2</v>
@@ -17544,13 +17565,13 @@
     </row>
     <row r="246" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B246" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C246" s="12" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D246" s="13">
         <v>16</v>
@@ -17608,13 +17629,13 @@
     </row>
     <row r="247" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B247" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C247" s="12" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="D247" s="13">
         <v>3</v>
@@ -17670,13 +17691,13 @@
     </row>
     <row r="248" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B248" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C248" s="12" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D248" s="13">
         <v>12</v>
@@ -17734,13 +17755,13 @@
     </row>
     <row r="249" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B249" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C249" s="12" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="D249" s="13">
         <v>1</v>
@@ -17798,13 +17819,13 @@
     </row>
     <row r="250" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B250" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C250" s="12" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D250" s="13">
         <v>1</v>
@@ -17862,13 +17883,13 @@
     </row>
     <row r="251" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B251" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C251" s="12" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D251" s="13">
         <v>2</v>
@@ -17926,13 +17947,13 @@
     </row>
     <row r="252" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B252" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C252" s="12" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D252" s="13">
         <v>1</v>
@@ -17990,13 +18011,13 @@
     </row>
     <row r="253" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B253" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C253" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D253" s="13">
         <v>19</v>
@@ -18054,13 +18075,13 @@
     </row>
     <row r="254" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B254" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C254" s="12" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D254" s="13">
         <v>6</v>
@@ -18118,13 +18139,13 @@
     </row>
     <row r="255" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B255" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C255" s="12" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D255" s="13">
         <v>1</v>
@@ -18182,13 +18203,13 @@
     </row>
     <row r="256" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B256" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C256" s="12" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D256" s="13">
         <v>15</v>
@@ -18246,13 +18267,13 @@
     </row>
     <row r="257" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B257" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C257" s="12" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D257" s="13">
         <v>5</v>
@@ -18310,13 +18331,13 @@
     </row>
     <row r="258" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B258" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D258" s="13">
         <v>1</v>
@@ -18374,13 +18395,13 @@
     </row>
     <row r="259" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B259" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="C259" s="12" t="s">
         <v>333</v>
-      </c>
-      <c r="C259" s="12" t="s">
-        <v>341</v>
       </c>
       <c r="D259" s="13">
         <v>7</v>
@@ -18438,13 +18459,13 @@
     </row>
     <row r="260" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B260" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C260" s="12" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D260" s="13">
         <v>8</v>
@@ -18502,13 +18523,13 @@
     </row>
     <row r="261" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B261" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C261" s="12" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="D261" s="13">
         <v>12</v>
@@ -18566,13 +18587,13 @@
     </row>
     <row r="262" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B262" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C262" s="12" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="D262" s="13">
         <v>68</v>
@@ -18630,13 +18651,13 @@
     </row>
     <row r="263" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B263" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C263" s="12" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D263" s="13">
         <v>4</v>
@@ -18694,13 +18715,13 @@
     </row>
     <row r="264" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="12" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B264" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C264" s="12" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="D264" s="13">
         <v>8</v>
@@ -18758,13 +18779,13 @@
     </row>
     <row r="265" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B265" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C265" s="12" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D265" s="13">
         <v>1</v>
@@ -18822,13 +18843,13 @@
     </row>
     <row r="266" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B266" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C266" s="12" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D266" s="13">
         <v>6</v>
@@ -18886,13 +18907,13 @@
     </row>
     <row r="267" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B267" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="D267" s="13">
         <v>2</v>
@@ -18950,13 +18971,13 @@
     </row>
     <row r="268" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B268" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C268" s="12" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="D268" s="13">
         <v>3</v>
@@ -19012,13 +19033,13 @@
     </row>
     <row r="269" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B269" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C269" s="12" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="D269" s="13">
         <v>1</v>
@@ -19076,13 +19097,13 @@
     </row>
     <row r="270" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B270" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C270" s="12" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D270" s="13">
         <v>22</v>
@@ -19140,13 +19161,13 @@
     </row>
     <row r="271" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B271" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C271" s="12" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D271" s="13">
         <v>3</v>
@@ -19202,13 +19223,13 @@
     </row>
     <row r="272" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="B272" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C272" s="12" t="s">
         <v>347</v>
-      </c>
-      <c r="B272" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C272" s="12" t="s">
-        <v>355</v>
       </c>
       <c r="D272" s="13">
         <v>1</v>
@@ -19266,13 +19287,13 @@
     </row>
     <row r="273" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B273" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C273" s="12" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D273" s="13">
         <v>6</v>
@@ -19330,13 +19351,13 @@
     </row>
     <row r="274" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B274" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C274" s="12" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D274" s="13">
         <v>2</v>
@@ -19394,13 +19415,13 @@
     </row>
     <row r="275" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B275" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D275" s="13">
         <v>3</v>
@@ -19456,13 +19477,13 @@
     </row>
     <row r="276" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B276" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D276" s="13">
         <v>2</v>
@@ -19520,13 +19541,13 @@
     </row>
     <row r="277" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B277" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C277" s="12" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D277" s="13">
         <v>3</v>
@@ -19582,13 +19603,13 @@
     </row>
     <row r="278" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B278" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C278" s="12" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D278" s="13">
         <v>6</v>
@@ -19646,13 +19667,13 @@
     </row>
     <row r="279" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B279" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C279" s="12" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D279" s="13">
         <v>6</v>
@@ -19710,13 +19731,13 @@
     </row>
     <row r="280" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B280" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C280" s="12" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D280" s="13">
         <v>2</v>
@@ -19774,13 +19795,13 @@
     </row>
     <row r="281" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B281" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C281" s="12" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D281" s="13">
         <v>23</v>
@@ -19838,13 +19859,13 @@
     </row>
     <row r="282" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B282" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C282" s="12" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D282" s="13">
         <v>1</v>
@@ -19902,13 +19923,13 @@
     </row>
     <row r="283" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B283" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C283" s="12" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="D283" s="13">
         <v>1</v>
@@ -19966,13 +19987,13 @@
     </row>
     <row r="284" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B284" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C284" s="12" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D284" s="13">
         <v>2</v>
@@ -20030,13 +20051,13 @@
     </row>
     <row r="285" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B285" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C285" s="12" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D285" s="13">
         <v>2</v>
@@ -20094,13 +20115,13 @@
     </row>
     <row r="286" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B286" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C286" s="12" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D286" s="13">
         <v>1</v>
@@ -20158,13 +20179,13 @@
     </row>
     <row r="287" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B287" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C287" s="12" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D287" s="13">
         <v>1</v>
@@ -20222,13 +20243,13 @@
     </row>
     <row r="288" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B288" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C288" s="12" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D288" s="13">
         <v>1</v>
@@ -20286,13 +20307,13 @@
     </row>
     <row r="289" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B289" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C289" s="12" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D289" s="13">
         <v>26</v>
@@ -20350,13 +20371,13 @@
     </row>
     <row r="290" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B290" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C290" s="12" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D290" s="13">
         <v>5</v>
@@ -20414,13 +20435,13 @@
     </row>
     <row r="291" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B291" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C291" s="12" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="D291" s="13">
         <v>5</v>
@@ -20478,13 +20499,13 @@
     </row>
     <row r="292" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B292" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C292" s="12" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="D292" s="13">
         <v>3</v>
@@ -20540,13 +20561,13 @@
     </row>
     <row r="293" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B293" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C293" s="12" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="D293" s="13">
         <v>2</v>
@@ -20604,13 +20625,13 @@
     </row>
     <row r="294" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B294" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C294" s="12" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="D294" s="13">
         <v>2</v>
@@ -20668,13 +20689,13 @@
     </row>
     <row r="295" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B295" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C295" s="12" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D295" s="13">
         <v>21</v>
@@ -20732,13 +20753,13 @@
     </row>
     <row r="296" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B296" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C296" s="12" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="D296" s="13">
         <v>6</v>
@@ -20796,13 +20817,13 @@
     </row>
     <row r="297" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B297" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="D297" s="13">
         <v>2</v>
@@ -20860,13 +20881,13 @@
     </row>
     <row r="298" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B298" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="D298" s="13">
         <v>2</v>
@@ -20924,13 +20945,13 @@
     </row>
     <row r="299" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B299" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C299" s="12" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="D299" s="13">
         <v>6</v>
@@ -20988,13 +21009,13 @@
     </row>
     <row r="300" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B300" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C300" s="12" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="D300" s="13">
         <v>1</v>
@@ -21052,13 +21073,13 @@
     </row>
     <row r="301" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B301" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C301" s="12" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="D301" s="13">
         <v>1</v>
@@ -21116,13 +21137,13 @@
     </row>
     <row r="302" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B302" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C302" s="12" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D302" s="13">
         <v>4</v>
@@ -21180,13 +21201,13 @@
     </row>
     <row r="303" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B303" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C303" s="12" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="D303" s="13">
         <v>3</v>
@@ -21242,13 +21263,13 @@
     </row>
     <row r="304" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B304" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C304" s="12" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D304" s="13">
         <v>1</v>
@@ -21306,13 +21327,13 @@
     </row>
     <row r="305" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B305" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C305" s="12" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="D305" s="13">
         <v>1</v>
@@ -21370,13 +21391,13 @@
     </row>
     <row r="306" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="B306" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C306" s="12" t="s">
         <v>381</v>
-      </c>
-      <c r="B306" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C306" s="12" t="s">
-        <v>389</v>
       </c>
       <c r="D306" s="13">
         <v>1</v>
@@ -21434,13 +21455,13 @@
     </row>
     <row r="307" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B307" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C307" s="12" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="D307" s="13">
         <v>4</v>
@@ -21498,13 +21519,13 @@
     </row>
     <row r="308" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B308" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C308" s="12" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="D308" s="13">
         <v>2</v>
@@ -21562,13 +21583,13 @@
     </row>
     <row r="309" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B309" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C309" s="12" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D309" s="13">
         <v>2</v>
@@ -21626,13 +21647,13 @@
     </row>
     <row r="310" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="12" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B310" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C310" s="12" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D310" s="13">
         <v>4</v>
@@ -21690,13 +21711,13 @@
     </row>
     <row r="311" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="12" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B311" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C311" s="12" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="D311" s="13">
         <v>1</v>
@@ -21754,13 +21775,13 @@
     </row>
     <row r="312" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="12" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B312" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C312" s="12" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="D312" s="13">
         <v>1</v>
@@ -21818,13 +21839,13 @@
     </row>
     <row r="313" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="12" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B313" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C313" s="12" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D313" s="13">
         <v>1</v>
@@ -21882,13 +21903,13 @@
     </row>
     <row r="314" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="12" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B314" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C314" s="12" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D314" s="13">
         <v>6</v>
@@ -21946,13 +21967,13 @@
     </row>
     <row r="315" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B315" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C315" s="12" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="D315" s="13">
         <v>6</v>
@@ -22010,13 +22031,13 @@
     </row>
     <row r="316" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B316" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C316" s="12" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D316" s="13">
         <v>1</v>
@@ -22074,13 +22095,13 @@
     </row>
     <row r="317" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B317" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C317" s="12" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D317" s="13">
         <v>5</v>
@@ -22138,13 +22159,13 @@
     </row>
     <row r="318" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B318" s="11" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C318" s="12" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="D318" s="13">
         <v>7</v>
@@ -22202,13 +22223,13 @@
     </row>
     <row r="319" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B319" s="11" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C319" s="12" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="D319" s="13">
         <v>2</v>
@@ -22266,13 +22287,13 @@
     </row>
     <row r="320" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="B320" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="C320" s="12" t="s">
         <v>399</v>
-      </c>
-      <c r="B320" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="C320" s="12" t="s">
-        <v>407</v>
       </c>
       <c r="D320" s="13">
         <v>2</v>
@@ -22330,13 +22351,13 @@
     </row>
     <row r="321" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B321" s="11" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C321" s="12" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="D321" s="13">
         <v>3</v>
@@ -22392,13 +22413,13 @@
     </row>
     <row r="322" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" s="12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B322" s="11" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C322" s="12" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D322" s="13">
         <v>18</v>
@@ -22456,13 +22477,13 @@
     </row>
     <row r="323" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="12" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B323" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C323" s="12" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D323" s="13">
         <v>1</v>
@@ -22520,13 +22541,13 @@
     </row>
     <row r="324" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="12" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B324" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C324" s="12" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D324" s="13">
         <v>4</v>

</xml_diff>